<commit_message>
📊 Relatório Atualizado: Sun Feb 15 06:35:16 UTC 2026
</commit_message>
<xml_diff>
--- a/Relatorio_RoboDerik_V70.xlsx
+++ b/Relatorio_RoboDerik_V70.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Data</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>15/02/2026 03:20:18</t>
+  </si>
+  <si>
+    <t>15/02/2026 06:35:16</t>
   </si>
   <si>
     <t>INICIO</t>
@@ -190,29 +193,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$A$2:$A$3</c:f>
+              <c:f>Performance!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Inicio</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>15/02/2026 03:20:18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15/02/2026 06:35:16</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$B$2:$B$3</c:f>
+              <c:f>Performance!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -326,29 +335,35 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$A$2:$A$3</c:f>
+              <c:f>Performance!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Inicio</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>15/02/2026 03:20:18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15/02/2026 06:35:16</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$E$2:$E$3</c:f>
+              <c:f>Performance!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -766,7 +781,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -819,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -842,7 +857,30 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>60.08</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>57.67</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Relatório Atualizado: Sun Feb 15 06:41:32 UTC 2026
</commit_message>
<xml_diff>
--- a/Relatorio_RoboDerik_V70.xlsx
+++ b/Relatorio_RoboDerik_V70.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Data</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>15/02/2026 06:35:16</t>
+  </si>
+  <si>
+    <t>15/02/2026 03:41:32</t>
   </si>
   <si>
     <t>INICIO</t>
@@ -163,7 +166,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Crescimento do Patrimônio (Juros Compostos)</a:t>
+              <a:t>Crescimento do Patrimônio</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -193,9 +196,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$A$2:$A$4</c:f>
+              <c:f>Performance!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Inicio</c:v>
                 </c:pt>
@@ -204,16 +207,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>15/02/2026 06:35:16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15/02/2026 03:41:32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$B$2:$B$4</c:f>
+              <c:f>Performance!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
                 </c:pt>
@@ -221,6 +227,9 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>60.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>60.08</c:v>
                 </c:pt>
               </c:numCache>
@@ -335,9 +344,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$A$2:$A$4</c:f>
+              <c:f>Performance!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Inicio</c:v>
                 </c:pt>
@@ -346,16 +355,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>15/02/2026 06:35:16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15/02/2026 03:41:32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$E$2:$E$4</c:f>
+              <c:f>Performance!$E$2:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -363,6 +375,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.08</c:v>
                 </c:pt>
               </c:numCache>
@@ -781,13 +796,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="5" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -834,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -857,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -880,7 +895,30 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>60.08</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>57.67</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Relatório Atualizado: Sun Feb 15 06:54:33 UTC 2026
</commit_message>
<xml_diff>
--- a/Relatorio_RoboDerik_V70.xlsx
+++ b/Relatorio_RoboDerik_V70.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Data</t>
   </si>
@@ -43,10 +43,13 @@
     <t>15/02/2026 03:20:18</t>
   </si>
   <si>
-    <t>15/02/2026 06:35:16</t>
+    <t>15/02/2026 03:35:16</t>
   </si>
   <si>
     <t>15/02/2026 03:41:32</t>
+  </si>
+  <si>
+    <t>15/02/2026 03:54:33</t>
   </si>
   <si>
     <t>INICIO</t>
@@ -196,9 +199,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$A$2:$A$5</c:f>
+              <c:f>Performance!$A$2:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Inicio</c:v>
                 </c:pt>
@@ -206,20 +209,23 @@
                   <c:v>15/02/2026 03:20:18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15/02/2026 06:35:16</c:v>
+                  <c:v>15/02/2026 03:35:16</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15/02/2026 03:41:32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15/02/2026 03:54:33</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$B$2:$B$5</c:f>
+              <c:f>Performance!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
                 </c:pt>
@@ -230,6 +236,9 @@
                   <c:v>60.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>60.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>60.08</c:v>
                 </c:pt>
               </c:numCache>
@@ -344,9 +353,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$A$2:$A$5</c:f>
+              <c:f>Performance!$A$2:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Inicio</c:v>
                 </c:pt>
@@ -354,20 +363,23 @@
                   <c:v>15/02/2026 03:20:18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15/02/2026 06:35:16</c:v>
+                  <c:v>15/02/2026 03:35:16</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15/02/2026 03:41:32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15/02/2026 03:54:33</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$E$2:$E$5</c:f>
+              <c:f>Performance!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -378,6 +390,9 @@
                   <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.08</c:v>
                 </c:pt>
               </c:numCache>
@@ -796,7 +811,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -849,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -872,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -895,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -918,7 +933,30 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>60.08</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>57.67</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>